<commit_message>
v 0.5.1 - test for measurments - back/cancel production sequenz - timer color
</commit_message>
<xml_diff>
--- a/FBGAcc_ProdutionsLog.xlsx
+++ b/FBGAcc_ProdutionsLog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Produktion Dokumentation</t>
   </si>
@@ -49,15 +49,6 @@
   </si>
   <si>
     <t>Vorspannung [nm]</t>
-  </si>
-  <si>
-    <t>Wellenlänge nach 8 min heiß  [nm]</t>
-  </si>
-  <si>
-    <t>Temperatur Rahmen nach 8 min [°C]</t>
-  </si>
-  <si>
-    <t>Wellenlänge nach Verklebung heiß (90°) [nm]</t>
   </si>
   <si>
     <t>Wellenlänge kalt LC/APC [nm]</t>
@@ -96,565 +87,10 @@
     <t>Halbwertsbreite -g [nm]</t>
   </si>
   <si>
-    <t>2016-0001</t>
+    <t>Wellenlänge vor Silikon  [nm]</t>
   </si>
   <si>
-    <t>Loptek(Fos4X)-1-26</t>
-  </si>
-  <si>
-    <t>0001</t>
-  </si>
-  <si>
-    <t>24.4</t>
-  </si>
-  <si>
-    <t>2016-0002</t>
-  </si>
-  <si>
-    <t>Loptek(Fos4X)-1-33</t>
-  </si>
-  <si>
-    <t>0002</t>
-  </si>
-  <si>
-    <t>24.2</t>
-  </si>
-  <si>
-    <t>2016-0003</t>
-  </si>
-  <si>
-    <t>Loptek(Fos4X)-1-22</t>
-  </si>
-  <si>
-    <t>0003</t>
-  </si>
-  <si>
-    <t>24.1</t>
-  </si>
-  <si>
-    <t>2016-0004</t>
-  </si>
-  <si>
-    <t>Loptek(Fos4X)-1-29</t>
-  </si>
-  <si>
-    <t>0004</t>
-  </si>
-  <si>
-    <t>23.9</t>
-  </si>
-  <si>
-    <t>2016-0005</t>
-  </si>
-  <si>
-    <t>Loptek(Fos4X)-1-21</t>
-  </si>
-  <si>
-    <t>0005</t>
-  </si>
-  <si>
-    <t>24.3</t>
-  </si>
-  <si>
-    <t>2016-0006</t>
-  </si>
-  <si>
-    <t>Loptek(Fos4X)-1-34</t>
-  </si>
-  <si>
-    <t>0006</t>
-  </si>
-  <si>
-    <t>23.6</t>
-  </si>
-  <si>
-    <t>2016-0007</t>
-  </si>
-  <si>
-    <t>Loptek(Fos4X)-1-27</t>
-  </si>
-  <si>
-    <t>0007</t>
-  </si>
-  <si>
-    <t>23.5</t>
-  </si>
-  <si>
-    <t>2016-0008</t>
-  </si>
-  <si>
-    <t>Loptek(Fos4X)-1-25</t>
-  </si>
-  <si>
-    <t>0008</t>
-  </si>
-  <si>
-    <t>23.7</t>
-  </si>
-  <si>
-    <t>2016-0009</t>
-  </si>
-  <si>
-    <t>Loptek(Fos4X)-1-30</t>
-  </si>
-  <si>
-    <t>0009</t>
-  </si>
-  <si>
-    <t>2016-0010</t>
-  </si>
-  <si>
-    <t>Loptek(Fos4X)-1-23</t>
-  </si>
-  <si>
-    <t>0010</t>
-  </si>
-  <si>
-    <t>2016-0011</t>
-  </si>
-  <si>
-    <t>Loptek(Fos4X)-1-24</t>
-  </si>
-  <si>
-    <t>0011</t>
-  </si>
-  <si>
-    <t>23.8</t>
-  </si>
-  <si>
-    <t>2016-0012</t>
-  </si>
-  <si>
-    <t>Loptek(Fos4X)-1-41</t>
-  </si>
-  <si>
-    <t>0012</t>
-  </si>
-  <si>
-    <t>20.05.2016</t>
-  </si>
-  <si>
-    <t>20160520_1106090012.spc</t>
-  </si>
-  <si>
-    <t>29.4</t>
-  </si>
-  <si>
-    <t>2016-0013</t>
-  </si>
-  <si>
-    <t>Loptek(Fox4x)-1-31</t>
-  </si>
-  <si>
-    <t>0013</t>
-  </si>
-  <si>
-    <t>20160520_1147160013.spc</t>
-  </si>
-  <si>
-    <t>30.0</t>
-  </si>
-  <si>
-    <t>2016-0014</t>
-  </si>
-  <si>
-    <t>Loptek(Fox4x)-1-47</t>
-  </si>
-  <si>
-    <t>0014</t>
-  </si>
-  <si>
-    <t>23.05.2016</t>
-  </si>
-  <si>
-    <t>20160523_1027490014.spc</t>
-  </si>
-  <si>
-    <t>29.7</t>
-  </si>
-  <si>
-    <t>2016-0015</t>
-  </si>
-  <si>
-    <t>Loptek(Fox4x)-1-18</t>
-  </si>
-  <si>
-    <t>0015</t>
-  </si>
-  <si>
-    <t>20160523_1105580015.spc</t>
-  </si>
-  <si>
-    <t>29.5</t>
-  </si>
-  <si>
-    <t>2016-0016</t>
-  </si>
-  <si>
-    <t>Loptek(Fox4x)-1-48</t>
-  </si>
-  <si>
-    <t>0016</t>
-  </si>
-  <si>
-    <t>20160523_1142360016.spc</t>
-  </si>
-  <si>
-    <t>30.6</t>
-  </si>
-  <si>
-    <t>2016-0017</t>
-  </si>
-  <si>
-    <t>Loptek(Fox4x)-1-44</t>
-  </si>
-  <si>
-    <t>0017</t>
-  </si>
-  <si>
-    <t>20160523_1208160017.spc</t>
-  </si>
-  <si>
-    <t>33.4</t>
-  </si>
-  <si>
-    <t>2016-0018</t>
-  </si>
-  <si>
-    <t>1-43</t>
-  </si>
-  <si>
-    <t>0018</t>
-  </si>
-  <si>
-    <t>20160523_1310360018.spc</t>
-  </si>
-  <si>
-    <t>29.3</t>
-  </si>
-  <si>
-    <t>2016-0019</t>
-  </si>
-  <si>
-    <t>1-36</t>
-  </si>
-  <si>
-    <t>0019</t>
-  </si>
-  <si>
-    <t>20160523_1350160019.spc</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>30.2</t>
-  </si>
-  <si>
-    <t>2016-0020</t>
-  </si>
-  <si>
-    <t>1-49</t>
-  </si>
-  <si>
-    <t>0020</t>
-  </si>
-  <si>
-    <t>20160523_1427540020.spc</t>
-  </si>
-  <si>
-    <t>2016-0021</t>
-  </si>
-  <si>
-    <t>1-42</t>
-  </si>
-  <si>
-    <t>0021</t>
-  </si>
-  <si>
-    <t>20160523_1449110021.spc</t>
-  </si>
-  <si>
-    <t>30.1</t>
-  </si>
-  <si>
-    <t>2016-0022</t>
-  </si>
-  <si>
-    <t>1-4</t>
-  </si>
-  <si>
-    <t>0022</t>
-  </si>
-  <si>
-    <t>06.06.2016</t>
-  </si>
-  <si>
-    <t>20160606_1025260022.spc</t>
-  </si>
-  <si>
-    <t>28.7</t>
-  </si>
-  <si>
-    <t>2016-0023</t>
-  </si>
-  <si>
-    <t>1-50</t>
-  </si>
-  <si>
-    <t>0023</t>
-  </si>
-  <si>
-    <t>20160606_1103390023.spc</t>
-  </si>
-  <si>
-    <t>27.8</t>
-  </si>
-  <si>
-    <t>2016-0024</t>
-  </si>
-  <si>
-    <t>1-6</t>
-  </si>
-  <si>
-    <t>0025</t>
-  </si>
-  <si>
-    <t>20160606_1143120025.spc</t>
-  </si>
-  <si>
-    <t>28.9</t>
-  </si>
-  <si>
-    <t>2016-0025</t>
-  </si>
-  <si>
-    <t>1-19</t>
-  </si>
-  <si>
-    <t>0027</t>
-  </si>
-  <si>
-    <t>20160606_1213190027.spc</t>
-  </si>
-  <si>
-    <t>2016-0026</t>
-  </si>
-  <si>
-    <t>1-5</t>
-  </si>
-  <si>
-    <t>0028</t>
-  </si>
-  <si>
-    <t>20160606_1317370028.spc</t>
-  </si>
-  <si>
-    <t>28.6</t>
-  </si>
-  <si>
-    <t>2016-0027</t>
-  </si>
-  <si>
-    <t>1-39</t>
-  </si>
-  <si>
-    <t>0029</t>
-  </si>
-  <si>
-    <t>20160606_1339550029.spc</t>
-  </si>
-  <si>
-    <t>28.3</t>
-  </si>
-  <si>
-    <t>2016-0028</t>
-  </si>
-  <si>
-    <t>1-3</t>
-  </si>
-  <si>
-    <t>0030</t>
-  </si>
-  <si>
-    <t>20160606_1405320030.spc</t>
-  </si>
-  <si>
-    <t>2016-0029</t>
-  </si>
-  <si>
-    <t>1-11</t>
-  </si>
-  <si>
-    <t>0031</t>
-  </si>
-  <si>
-    <t>20160606_1424200031.spc</t>
-  </si>
-  <si>
-    <t>28.8</t>
-  </si>
-  <si>
-    <t>2016-0030</t>
-  </si>
-  <si>
-    <t>1-28</t>
-  </si>
-  <si>
-    <t>0032</t>
-  </si>
-  <si>
-    <t>20160606_1446090032.spc</t>
-  </si>
-  <si>
-    <t>29.1</t>
-  </si>
-  <si>
-    <t>2016-0031</t>
-  </si>
-  <si>
-    <t>1-38</t>
-  </si>
-  <si>
-    <t>0033</t>
-  </si>
-  <si>
-    <t>20160606_1504020033.spc</t>
-  </si>
-  <si>
-    <t>2016-0032</t>
-  </si>
-  <si>
-    <t>1-35</t>
-  </si>
-  <si>
-    <t>0034</t>
-  </si>
-  <si>
-    <t>07.06.2016</t>
-  </si>
-  <si>
-    <t>20160607_0816180034.spc</t>
-  </si>
-  <si>
-    <t>2016-0033</t>
-  </si>
-  <si>
-    <t>1-45</t>
-  </si>
-  <si>
-    <t>0036</t>
-  </si>
-  <si>
-    <t>20160607_0847120036.spc</t>
-  </si>
-  <si>
-    <t>2016-0034</t>
-  </si>
-  <si>
-    <t>1-17</t>
-  </si>
-  <si>
-    <t>0037</t>
-  </si>
-  <si>
-    <t>20160607_0942080037.spc</t>
-  </si>
-  <si>
-    <t>2016-0035</t>
-  </si>
-  <si>
-    <t>1-32</t>
-  </si>
-  <si>
-    <t>0038</t>
-  </si>
-  <si>
-    <t>20160607_1011580038.spc</t>
-  </si>
-  <si>
-    <t>2016-0036</t>
-  </si>
-  <si>
-    <t>1-40</t>
-  </si>
-  <si>
-    <t>0039</t>
-  </si>
-  <si>
-    <t>20160607_1041590039.spc</t>
-  </si>
-  <si>
-    <t>2016-0037</t>
-  </si>
-  <si>
-    <t>1-37</t>
-  </si>
-  <si>
-    <t>0040</t>
-  </si>
-  <si>
-    <t>20160607_1121530040.spc</t>
-  </si>
-  <si>
-    <t>2016-0038</t>
-  </si>
-  <si>
-    <t>1-1</t>
-  </si>
-  <si>
-    <t>0041</t>
-  </si>
-  <si>
-    <t>20160607_1152220041.spc</t>
-  </si>
-  <si>
-    <t>2016-0039</t>
-  </si>
-  <si>
-    <t>1-2</t>
-  </si>
-  <si>
-    <t>0042</t>
-  </si>
-  <si>
-    <t>20160607_1220220042.spc</t>
-  </si>
-  <si>
-    <t>2016-0040</t>
-  </si>
-  <si>
-    <t>1-8</t>
-  </si>
-  <si>
-    <t>0043</t>
-  </si>
-  <si>
-    <t>20160607_1313470043.spc</t>
-  </si>
-  <si>
-    <t>2016-0041</t>
-  </si>
-  <si>
-    <t>1-9</t>
-  </si>
-  <si>
-    <t>0044</t>
-  </si>
-  <si>
-    <t>20160607_1346290044.spc</t>
-  </si>
-  <si>
-    <t>2016-0042</t>
-  </si>
-  <si>
-    <t>1-15</t>
-  </si>
-  <si>
-    <t>0045</t>
-  </si>
-  <si>
-    <t>20160607_1412550045.spc</t>
+    <t>Wellenlänge nach Silikon  [nm]</t>
   </si>
 </sst>
 </file>
@@ -1098,8 +534,8 @@
   </sheetPr>
   <dimension ref="A2:AA1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:E49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,8 +549,7 @@
     <col min="7" max="7" width="8" style="1" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="7.42578125" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="8.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="1" customWidth="1"/>
-    <col min="11" max="13" width="9.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="13" width="9.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" customWidth="1"/>
     <col min="15" max="16" width="9.140625" style="1" customWidth="1"/>
     <col min="17" max="20" width="9.140625" style="8" customWidth="1"/>
@@ -1162,2518 +597,968 @@
         <v>6</v>
       </c>
       <c r="L4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="Q4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="R4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="Z4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="AA4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="6">
-        <v>42409</v>
-      </c>
-      <c r="E5" s="9">
-        <v>1545.0609999999999</v>
-      </c>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="9">
-        <v>1553.4780000000001</v>
-      </c>
+      <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
-      <c r="N5" s="9">
-        <v>1551.7</v>
-      </c>
-      <c r="O5" s="9">
-        <v>1550.1679999999999</v>
-      </c>
-      <c r="P5" s="9">
-        <f t="shared" ref="P5:P68" si="0">IF(O5,O5-1550,"-")</f>
-        <v>0.16799999999989268</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="R5" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="S5" s="7">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="T5" s="7">
-        <v>1550.5530000000001</v>
-      </c>
-      <c r="U5" s="9">
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="V5" s="9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="W5" s="9">
-        <v>0.53400000000000003</v>
-      </c>
-      <c r="X5" s="9">
-        <v>1549.816</v>
-      </c>
-      <c r="Y5" s="9">
-        <v>0.35199999999999998</v>
-      </c>
-      <c r="Z5" s="9">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="AA5" s="9">
-        <v>0.53100000000000003</v>
-      </c>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="6">
-        <v>42409</v>
-      </c>
-      <c r="E6" s="9">
-        <v>1554.1220000000001</v>
-      </c>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="9">
-        <v>1553.373</v>
-      </c>
+      <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="9">
-        <v>1551.4770000000001</v>
-      </c>
-      <c r="O6" s="9">
-        <v>1550.502</v>
-      </c>
-      <c r="P6" s="9">
-        <f t="shared" si="0"/>
-        <v>0.50199999999995271</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="7">
-        <v>0</v>
-      </c>
-      <c r="S6" s="7">
-        <v>0.53100000000000003</v>
-      </c>
-      <c r="T6" s="7">
-        <v>1550.86</v>
-      </c>
-      <c r="U6" s="9">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="V6" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="W6" s="9">
-        <v>0.52300000000000002</v>
-      </c>
-      <c r="X6" s="9">
-        <v>1550.16</v>
-      </c>
-      <c r="Y6" s="9">
-        <v>0.34200000000000003</v>
-      </c>
-      <c r="Z6" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="AA6" s="9">
-        <v>0.53</v>
-      </c>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="6">
-        <v>42410</v>
-      </c>
-      <c r="E7" s="9">
-        <v>1545.06</v>
-      </c>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="9">
-        <v>1553.502</v>
-      </c>
+      <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="9">
-        <v>1551.6</v>
-      </c>
-      <c r="O7" s="9">
-        <v>1550.1590000000001</v>
-      </c>
-      <c r="P7" s="9">
-        <f t="shared" si="0"/>
-        <v>0.1590000000001055</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="R7" s="7">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="S7" s="7">
-        <v>0.55800000000000005</v>
-      </c>
-      <c r="T7" s="7">
-        <v>1550.625</v>
-      </c>
-      <c r="U7" s="9">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="V7" s="9">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="W7" s="9">
-        <v>0.55300000000000005</v>
-      </c>
-      <c r="X7" s="9">
-        <v>1549.7329999999999</v>
-      </c>
-      <c r="Y7" s="9">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="Z7" s="9">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="AA7" s="9">
-        <v>0.55300000000000005</v>
-      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="6">
-        <v>42410</v>
-      </c>
-      <c r="E8" s="9">
-        <v>1545.203</v>
-      </c>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="9">
-        <v>1553.5</v>
-      </c>
+      <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="9">
-        <v>1551.29</v>
-      </c>
-      <c r="O8" s="9">
-        <v>1550.856</v>
-      </c>
-      <c r="P8" s="9">
-        <f t="shared" si="0"/>
-        <v>0.85599999999999454</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="R8" s="7">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="S8" s="7">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="T8" s="7">
-        <v>1551.2539999999999</v>
-      </c>
-      <c r="U8" s="9">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="V8" s="9">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="W8" s="9">
-        <v>0.52800000000000002</v>
-      </c>
-      <c r="X8" s="9">
-        <v>1550.502</v>
-      </c>
-      <c r="Y8" s="9">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="Z8" s="9">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="AA8" s="9">
-        <v>0.52800000000000002</v>
-      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="6">
-        <v>42410</v>
-      </c>
-      <c r="E9" s="9">
-        <v>1545.0630000000001</v>
-      </c>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="9">
-        <v>1553.5060000000001</v>
-      </c>
+      <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="9">
-        <v>1551.75</v>
-      </c>
-      <c r="O9" s="9">
-        <v>1550.252</v>
-      </c>
-      <c r="P9" s="9">
-        <f t="shared" si="0"/>
-        <v>0.25199999999995271</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="R9" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="S9" s="7">
-        <v>0.54100000000000004</v>
-      </c>
-      <c r="T9" s="7">
-        <v>1550.693</v>
-      </c>
-      <c r="U9" s="9">
-        <v>0.441</v>
-      </c>
-      <c r="V9" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="W9" s="9">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="X9" s="9">
-        <v>1549.8440000000001</v>
-      </c>
-      <c r="Y9" s="9">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="Z9" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AA9" s="9">
-        <v>0.53900000000000003</v>
-      </c>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="6">
-        <v>42410</v>
-      </c>
-      <c r="E10" s="9">
-        <v>1545.21</v>
-      </c>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="9">
-        <v>1553.5039999999999</v>
-      </c>
+      <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="9">
-        <v>1552.2</v>
-      </c>
-      <c r="O10" s="9">
-        <v>1550.6679999999999</v>
-      </c>
-      <c r="P10" s="9">
-        <f t="shared" si="0"/>
-        <v>0.66799999999989268</v>
-      </c>
-      <c r="Q10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="R10" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="S10" s="7">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="T10" s="7">
-        <v>1551.077</v>
-      </c>
-      <c r="U10" s="9">
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="V10" s="9">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="W10" s="9">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="X10" s="9">
-        <v>1550.27</v>
-      </c>
-      <c r="Y10" s="9">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="Z10" s="9">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="AA10" s="9">
-        <v>0.52200000000000002</v>
-      </c>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="6">
-        <v>42416</v>
-      </c>
-      <c r="E11" s="9">
-        <v>1545.0260000000001</v>
-      </c>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="9">
-        <v>1553.585</v>
-      </c>
+      <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
-      <c r="N11" s="9">
-        <v>1552.94</v>
-      </c>
-      <c r="O11" s="9">
-        <v>1550.5809999999999</v>
-      </c>
-      <c r="P11" s="9">
-        <f t="shared" si="0"/>
-        <v>0.58099999999990359</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="R11" s="7">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="S11" s="7">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="T11" s="7">
-        <v>1551.056</v>
-      </c>
-      <c r="U11" s="9">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="V11" s="9">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="W11" s="9">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="X11" s="9">
-        <v>1550.123</v>
-      </c>
-      <c r="Y11" s="9">
-        <v>0.45800000000000002</v>
-      </c>
-      <c r="Z11" s="9">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="AA11" s="9">
-        <v>0.53900000000000003</v>
-      </c>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="6">
-        <v>42416</v>
-      </c>
-      <c r="E12" s="9">
-        <v>1545.08</v>
-      </c>
-      <c r="F12" s="9">
-        <v>30.8</v>
-      </c>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="9">
-        <v>1553.5820000000001</v>
-      </c>
+      <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
-      <c r="N12" s="9">
-        <v>1552.45</v>
-      </c>
-      <c r="O12" s="9">
-        <v>1550.7239999999999</v>
-      </c>
-      <c r="P12" s="9">
-        <f t="shared" si="0"/>
-        <v>0.7239999999999327</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="R12" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="S12" s="7">
-        <v>0.56299999999999994</v>
-      </c>
-      <c r="T12" s="7">
-        <v>1551.1210000000001</v>
-      </c>
-      <c r="U12" s="9">
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="V12" s="9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="W12" s="9">
-        <v>0.56299999999999994</v>
-      </c>
-      <c r="X12" s="9">
-        <v>1550.3620000000001</v>
-      </c>
-      <c r="Y12" s="9">
-        <v>0.36199999999999999</v>
-      </c>
-      <c r="Z12" s="9">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="AA12" s="9">
-        <v>0.56299999999999994</v>
-      </c>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="6">
-        <v>42416</v>
-      </c>
-      <c r="E13" s="9">
-        <v>1545.06</v>
-      </c>
-      <c r="F13" s="9">
-        <v>25</v>
-      </c>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="9">
-        <v>1553.5840000000001</v>
-      </c>
+      <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="9">
-        <v>1552.9</v>
-      </c>
-      <c r="O13" s="9">
-        <v>1551.2280000000001</v>
-      </c>
-      <c r="P13" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2280000000000655</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="R13" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="S13" s="7">
-        <v>0.52300000000000002</v>
-      </c>
-      <c r="T13" s="7">
-        <v>1551.6510000000001</v>
-      </c>
-      <c r="U13" s="9">
-        <v>0.42299999999999999</v>
-      </c>
-      <c r="V13" s="9">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="W13" s="9">
-        <v>0.52900000000000003</v>
-      </c>
-      <c r="X13" s="9">
-        <v>1550.8409999999999</v>
-      </c>
-      <c r="Y13" s="9">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="Z13" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AA13" s="9">
-        <v>0.51900000000000002</v>
-      </c>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="6">
-        <v>42416</v>
-      </c>
-      <c r="E14" s="9">
-        <v>1545.17</v>
-      </c>
-      <c r="F14" s="9">
-        <v>27.6</v>
-      </c>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="9">
-        <v>1553.57</v>
-      </c>
+      <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
-      <c r="N14" s="9">
-        <v>1552.3</v>
-      </c>
-      <c r="O14" s="9">
-        <v>1550.854</v>
-      </c>
-      <c r="P14" s="9">
-        <f t="shared" si="0"/>
-        <v>0.85400000000004184</v>
-      </c>
-      <c r="Q14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="R14" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="S14" s="7">
-        <v>0.55900000000000005</v>
-      </c>
-      <c r="T14" s="7">
-        <v>1551.231</v>
-      </c>
-      <c r="U14" s="9">
-        <v>0.377</v>
-      </c>
-      <c r="V14" s="9">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="W14" s="9">
-        <v>0.56499999999999995</v>
-      </c>
-      <c r="X14" s="9">
-        <v>1550.4960000000001</v>
-      </c>
-      <c r="Y14" s="9">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="Z14" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="AA14" s="9">
-        <v>0.56699999999999995</v>
-      </c>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="6">
-        <v>42416</v>
-      </c>
-      <c r="E15" s="9">
-        <v>1545.11</v>
-      </c>
-      <c r="F15" s="9">
-        <v>29.1</v>
-      </c>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="9">
-        <v>1553.644</v>
-      </c>
+      <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="9">
-        <v>1552.67</v>
-      </c>
-      <c r="O15" s="9">
-        <v>1550.2570000000001</v>
-      </c>
-      <c r="P15" s="9">
-        <f t="shared" si="0"/>
-        <v>0.25700000000006185</v>
-      </c>
-      <c r="Q15" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="R15" s="7">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="S15" s="7">
-        <v>0.53300000000000003</v>
-      </c>
-      <c r="T15" s="7">
-        <v>1550.6</v>
-      </c>
-      <c r="U15" s="9">
-        <v>0.34300000000000003</v>
-      </c>
-      <c r="V15" s="9">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="W15" s="9">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="X15" s="9">
-        <v>1549.9369999999999</v>
-      </c>
-      <c r="Y15" s="9">
-        <v>0.32</v>
-      </c>
-      <c r="Z15" s="9">
-        <v>2E-3</v>
-      </c>
-      <c r="AA15" s="9">
-        <v>0.53500000000000003</v>
-      </c>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="9">
-        <v>1545.0709999999999</v>
-      </c>
-      <c r="F16" s="9">
-        <v>25.3</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H16" s="9">
-        <v>0.6340110438845149</v>
-      </c>
-      <c r="I16" s="9">
-        <v>6.1534700098491157E-3</v>
-      </c>
-      <c r="J16" s="9">
-        <v>1553.046</v>
-      </c>
-      <c r="K16" s="9">
-        <v>25.3</v>
-      </c>
-      <c r="L16" s="9">
-        <v>1554.816</v>
-      </c>
-      <c r="M16" s="9">
-        <v>156.9</v>
-      </c>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="9">
-        <v>1551.0129999999999</v>
-      </c>
-      <c r="P16" s="9">
-        <f t="shared" si="0"/>
-        <v>1.01299999999992</v>
-      </c>
-      <c r="Q16" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="R16" s="7">
-        <v>0</v>
-      </c>
-      <c r="S16" s="7">
-        <v>0.52700000000000002</v>
-      </c>
-      <c r="T16" s="7">
-        <v>1551.5260000000001</v>
-      </c>
-      <c r="U16" s="9">
-        <v>0.51300000000000001</v>
-      </c>
-      <c r="V16" s="9">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="W16" s="9">
-        <v>0.53300000000000003</v>
-      </c>
-      <c r="X16" s="9">
-        <v>1550.5119999999999</v>
-      </c>
-      <c r="Y16" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="Z16" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="AA16" s="9">
-        <v>0.53500000000000003</v>
-      </c>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="9">
-        <v>1545.0930000000001</v>
-      </c>
-      <c r="F17" s="9">
-        <v>33.9</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" s="9">
-        <v>0.54524410152347558</v>
-      </c>
-      <c r="I17" s="9">
-        <v>6.0817866128672904E-3</v>
-      </c>
-      <c r="J17" s="9">
-        <v>1553.039</v>
-      </c>
-      <c r="K17" s="9">
-        <v>33.200000000000003</v>
-      </c>
-      <c r="L17" s="9">
-        <v>1555.309</v>
-      </c>
-      <c r="M17" s="9">
-        <v>140.5</v>
-      </c>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="9">
-        <v>1550.54</v>
-      </c>
-      <c r="P17" s="9">
-        <f t="shared" si="0"/>
-        <v>0.53999999999996362</v>
-      </c>
-      <c r="Q17" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="R17" s="7">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="S17" s="7">
-        <v>0.53900000000000003</v>
-      </c>
-      <c r="T17" s="7">
-        <v>1550.943</v>
-      </c>
-      <c r="U17" s="9">
-        <v>0.40400000000000003</v>
-      </c>
-      <c r="V17" s="9">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="W17" s="9">
-        <v>0.53900000000000003</v>
-      </c>
-      <c r="X17" s="9">
-        <v>1550.1379999999999</v>
-      </c>
-      <c r="Y17" s="9">
-        <v>0.40100000000000002</v>
-      </c>
-      <c r="Z17" s="9">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="AA17" s="9">
-        <v>0.53600000000000003</v>
-      </c>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="9">
-        <v>1545.124</v>
-      </c>
-      <c r="F18" s="9">
-        <v>28</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="H18" s="9">
-        <v>0.72137943023865414</v>
-      </c>
-      <c r="I18" s="9">
-        <v>2.9407451372662759E-3</v>
-      </c>
-      <c r="J18" s="9">
-        <v>1553.0429999999999</v>
-      </c>
-      <c r="K18" s="9">
-        <v>28</v>
-      </c>
-      <c r="L18" s="9">
-        <v>1555.114</v>
-      </c>
-      <c r="M18" s="9">
-        <v>148.19999999999999</v>
-      </c>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="9">
-        <v>1550.1179999999999</v>
-      </c>
-      <c r="P18" s="9">
-        <f t="shared" si="0"/>
-        <v>0.11799999999993815</v>
-      </c>
-      <c r="Q18" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="R18" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="S18" s="7">
-        <v>0.56100000000000005</v>
-      </c>
-      <c r="T18" s="7">
-        <v>1550.54</v>
-      </c>
-      <c r="U18" s="9">
-        <v>0.42199999999999999</v>
-      </c>
-      <c r="V18" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="W18" s="9">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="X18" s="9">
-        <v>1549.6849999999999</v>
-      </c>
-      <c r="Y18" s="9">
-        <v>0.433</v>
-      </c>
-      <c r="Z18" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="AA18" s="9">
-        <v>0.56299999999999994</v>
-      </c>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="9">
-        <v>1545.1949999999999</v>
-      </c>
-      <c r="F19" s="9">
-        <v>37.6</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="H19" s="9">
-        <v>0.97000834157021798</v>
-      </c>
-      <c r="I19" s="9">
-        <v>2.6920322109162949E-3</v>
-      </c>
-      <c r="J19" s="9">
-        <v>1553.086</v>
-      </c>
-      <c r="K19" s="9">
-        <v>37.1</v>
-      </c>
-      <c r="L19" s="9">
-        <v>1555.241</v>
-      </c>
-      <c r="M19" s="9">
-        <v>159.19999999999999</v>
-      </c>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="9">
-        <v>1551.2</v>
-      </c>
-      <c r="P19" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2000000000000455</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="R19" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="S19" s="7">
-        <v>0.56899999999999995</v>
-      </c>
-      <c r="T19" s="7">
-        <v>1551.6310000000001</v>
-      </c>
-      <c r="U19" s="9">
-        <v>0.432</v>
-      </c>
-      <c r="V19" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="W19" s="9">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="X19" s="9">
-        <v>1550.742</v>
-      </c>
-      <c r="Y19" s="9">
-        <v>0.45800000000000002</v>
-      </c>
-      <c r="Z19" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="AA19" s="9">
-        <v>0.56999999999999995</v>
-      </c>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="9">
-        <v>1545.202</v>
-      </c>
-      <c r="F20" s="9">
-        <v>36.1</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" s="9">
-        <v>0.75642738283234356</v>
-      </c>
-      <c r="I20" s="9">
-        <v>3.5731660052533698E-3</v>
-      </c>
-      <c r="J20" s="9">
-        <v>1553.002</v>
-      </c>
-      <c r="K20" s="9">
-        <v>35.6</v>
-      </c>
-      <c r="L20" s="9">
-        <v>1555.1320000000001</v>
-      </c>
-      <c r="M20" s="9">
-        <v>152.69999999999999</v>
-      </c>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="9">
-        <v>1551.316</v>
-      </c>
-      <c r="P20" s="9">
-        <f t="shared" si="0"/>
-        <v>1.3160000000000309</v>
-      </c>
-      <c r="Q20" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="R20" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="S20" s="7">
-        <v>0.55900000000000005</v>
-      </c>
-      <c r="T20" s="7">
-        <v>1551.7239999999999</v>
-      </c>
-      <c r="U20" s="9">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="V20" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="W20" s="9">
-        <v>0.56399999999999995</v>
-      </c>
-      <c r="X20" s="9">
-        <v>1550.89</v>
-      </c>
-      <c r="Y20" s="9">
-        <v>0.42599999999999999</v>
-      </c>
-      <c r="Z20" s="9">
-        <v>2E-3</v>
-      </c>
-      <c r="AA20" s="9">
-        <v>0.56299999999999994</v>
-      </c>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="9">
-        <v>1545.191</v>
-      </c>
-      <c r="F21" s="9">
-        <v>43.7</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="H21" s="9">
-        <v>0.76736004669894142</v>
-      </c>
-      <c r="I21" s="9">
-        <v>2.2118344393220468E-3</v>
-      </c>
-      <c r="J21" s="9">
-        <v>1553.0129999999999</v>
-      </c>
-      <c r="K21" s="9">
-        <v>42.9</v>
-      </c>
-      <c r="L21" s="9">
-        <v>1554.933</v>
-      </c>
-      <c r="M21" s="9">
-        <v>149.4</v>
-      </c>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="9">
-        <v>1550.087</v>
-      </c>
-      <c r="P21" s="9">
-        <f t="shared" si="0"/>
-        <v>8.6999999999989086E-2</v>
-      </c>
-      <c r="Q21" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="R21" s="7">
-        <v>2E-3</v>
-      </c>
-      <c r="S21" s="7">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="T21" s="7">
-        <v>1550.481</v>
-      </c>
-      <c r="U21" s="9">
-        <v>0.39400000000000002</v>
-      </c>
-      <c r="V21" s="9">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="W21" s="9">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="X21" s="9">
-        <v>1549.704</v>
-      </c>
-      <c r="Y21" s="9">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="Z21" s="9">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="AA21" s="9">
-        <v>0.55900000000000005</v>
-      </c>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="9">
-        <v>1545.19</v>
-      </c>
-      <c r="F22" s="9">
-        <v>31.4</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="H22" s="9">
-        <v>0.7416818033993775</v>
-      </c>
-      <c r="I22" s="9">
-        <v>7.6596960248025434E-3</v>
-      </c>
-      <c r="J22" s="9">
-        <v>1553.0229999999999</v>
-      </c>
-      <c r="K22" s="9">
-        <v>31.6</v>
-      </c>
-      <c r="L22" s="9">
-        <v>1555.078</v>
-      </c>
-      <c r="M22" s="9">
-        <v>155.4</v>
-      </c>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="9">
-        <v>1549.9590000000001</v>
-      </c>
-      <c r="P22" s="9">
-        <f t="shared" si="0"/>
-        <v>-4.0999999999939973E-2</v>
-      </c>
-      <c r="Q22" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="R22" s="7">
-        <v>2E-3</v>
-      </c>
-      <c r="S22" s="7">
-        <v>0.56499999999999995</v>
-      </c>
-      <c r="T22" s="7">
-        <v>1550.4059999999999</v>
-      </c>
-      <c r="U22" s="9">
-        <v>0.44700000000000001</v>
-      </c>
-      <c r="V22" s="9">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="W22" s="9">
-        <v>0.56699999999999995</v>
-      </c>
-      <c r="X22" s="9">
-        <v>1549.5160000000001</v>
-      </c>
-      <c r="Y22" s="9">
-        <v>0.442</v>
-      </c>
-      <c r="Z22" s="9">
-        <v>2E-3</v>
-      </c>
-      <c r="AA22" s="9">
-        <v>0.56699999999999995</v>
-      </c>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="9">
-        <v>0</v>
-      </c>
-      <c r="F23" s="9">
-        <v>39.299999999999997</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="H23" s="9">
-        <v>0.76277457608537325</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="J23" s="9">
-        <v>1553.0609999999999</v>
-      </c>
-      <c r="K23" s="9">
-        <v>37.799999999999997</v>
-      </c>
-      <c r="L23" s="9">
-        <v>1555.0989999999999</v>
-      </c>
-      <c r="M23" s="9">
-        <v>148</v>
-      </c>
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="9">
-        <v>1548.644</v>
-      </c>
-      <c r="P23" s="9">
-        <f t="shared" si="0"/>
-        <v>-1.3559999999999945</v>
-      </c>
-      <c r="Q23" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="R23" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="S23" s="7">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="T23" s="7">
-        <v>1549.0740000000001</v>
-      </c>
-      <c r="U23" s="9">
-        <v>0.42899999999999999</v>
-      </c>
-      <c r="V23" s="9">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="W23" s="9">
-        <v>0.51700000000000002</v>
-      </c>
-      <c r="X23" s="9">
-        <v>1548.2560000000001</v>
-      </c>
-      <c r="Y23" s="9">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="Z23" s="9">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="AA23" s="9">
-        <v>0.51300000000000001</v>
-      </c>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="9">
-        <v>1545.259</v>
-      </c>
-      <c r="F24" s="9">
-        <v>38.4</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="H24" s="9">
-        <v>0.76488732147139438</v>
-      </c>
-      <c r="I24" s="9">
-        <v>9.3305028826762282E-4</v>
-      </c>
-      <c r="J24" s="9">
-        <v>1553.037</v>
-      </c>
-      <c r="K24" s="9">
-        <v>37.799999999999997</v>
-      </c>
-      <c r="L24" s="9">
-        <v>1554.8489999999999</v>
-      </c>
-      <c r="M24" s="9">
-        <v>148.4</v>
-      </c>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="9">
-        <v>1550.0509999999999</v>
-      </c>
-      <c r="P24" s="9">
-        <f t="shared" si="0"/>
-        <v>5.0999999999930878E-2</v>
-      </c>
-      <c r="Q24" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="R24" s="7">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="S24" s="7">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="T24" s="7">
-        <v>1550.395</v>
-      </c>
-      <c r="U24" s="9">
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="V24" s="9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="W24" s="9">
-        <v>0.56299999999999994</v>
-      </c>
-      <c r="X24" s="9">
-        <v>1549.6759999999999</v>
-      </c>
-      <c r="Y24" s="9">
-        <v>0.374</v>
-      </c>
-      <c r="Z24" s="9">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="AA24" s="9">
-        <v>0.56499999999999995</v>
-      </c>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="9">
-        <v>1545.2840000000001</v>
-      </c>
-      <c r="F25" s="9">
-        <v>42.9</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H25" s="9">
-        <v>0.76861392806272644</v>
-      </c>
-      <c r="I25" s="9">
-        <v>2.619741153239374E-3</v>
-      </c>
-      <c r="J25" s="9">
-        <v>1553.0440000000001</v>
-      </c>
-      <c r="K25" s="9">
-        <v>42.7</v>
-      </c>
-      <c r="L25" s="9">
-        <v>1554.94</v>
-      </c>
-      <c r="M25" s="9">
-        <v>153.1</v>
-      </c>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="9">
-        <v>1551.374</v>
-      </c>
-      <c r="P25" s="9">
-        <f t="shared" si="0"/>
-        <v>1.3740000000000236</v>
-      </c>
-      <c r="Q25" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="R25" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="S25" s="7">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="T25" s="7">
-        <v>1551.7429999999999</v>
-      </c>
-      <c r="U25" s="9">
-        <v>0.36899999999999999</v>
-      </c>
-      <c r="V25" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="W25" s="9">
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="X25" s="9">
-        <v>1550.9760000000001</v>
-      </c>
-      <c r="Y25" s="9">
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="Z25" s="9">
-        <v>2E-3</v>
-      </c>
-      <c r="AA25" s="9">
-        <v>0.56599999999999995</v>
-      </c>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E26" s="9">
-        <v>1544.9849999999999</v>
-      </c>
-      <c r="F26" s="9">
-        <v>28.9</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="H26" s="9">
-        <v>0.71871229770789791</v>
-      </c>
-      <c r="I26" s="9">
-        <v>4.9497517736654117E-3</v>
-      </c>
-      <c r="J26" s="9">
-        <v>1552.944</v>
-      </c>
-      <c r="K26" s="9">
-        <v>29.1</v>
-      </c>
-      <c r="L26" s="9">
-        <v>1554.9059999999999</v>
-      </c>
-      <c r="M26" s="9">
-        <v>148.5</v>
-      </c>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
       <c r="N26" s="9"/>
-      <c r="O26" s="9">
-        <v>1549.6189999999999</v>
-      </c>
-      <c r="P26" s="9">
-        <f t="shared" si="0"/>
-        <v>-0.38100000000008549</v>
-      </c>
-      <c r="Q26" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="R26" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="S26" s="7">
-        <v>0.61099999999999999</v>
-      </c>
-      <c r="T26" s="7">
-        <v>1550.1579999999999</v>
-      </c>
-      <c r="U26" s="9">
-        <v>0.53900000000000003</v>
-      </c>
-      <c r="V26" s="9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="W26" s="9">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="X26" s="9">
-        <v>1549.088</v>
-      </c>
-      <c r="Y26" s="9">
-        <v>0.53100000000000003</v>
-      </c>
-      <c r="Z26" s="9">
-        <v>2E-3</v>
-      </c>
-      <c r="AA26" s="9">
-        <v>0.61199999999999999</v>
-      </c>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E27" s="9">
-        <v>1545.1890000000001</v>
-      </c>
-      <c r="F27" s="9">
-        <v>39.4</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="H27" s="9">
-        <v>0.63856657281892248</v>
-      </c>
-      <c r="I27" s="9">
-        <v>2.8135350171396571E-3</v>
-      </c>
-      <c r="J27" s="9">
-        <v>1552.9449999999999</v>
-      </c>
-      <c r="K27" s="9">
-        <v>39</v>
-      </c>
-      <c r="L27" s="9">
-        <v>1553.588</v>
-      </c>
-      <c r="M27" s="9">
-        <v>150.19999999999999</v>
-      </c>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
       <c r="N27" s="9"/>
-      <c r="O27" s="9">
-        <v>1549.94</v>
-      </c>
-      <c r="P27" s="9">
-        <f t="shared" si="0"/>
-        <v>-5.999999999994543E-2</v>
-      </c>
-      <c r="Q27" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="R27" s="7">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="S27" s="7">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="T27" s="7">
-        <v>1550.453</v>
-      </c>
-      <c r="U27" s="9">
-        <v>0.51300000000000001</v>
-      </c>
-      <c r="V27" s="9">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="W27" s="9">
-        <v>0.56499999999999995</v>
-      </c>
-      <c r="X27" s="9">
-        <v>1549.451</v>
-      </c>
-      <c r="Y27" s="9">
-        <v>0.49</v>
-      </c>
-      <c r="Z27" s="9">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="AA27" s="9">
-        <v>0.56499999999999995</v>
-      </c>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E28" s="9">
-        <v>1545.21</v>
-      </c>
-      <c r="F28" s="9">
-        <v>38.4</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="H28" s="9">
-        <v>0.64413772156959725</v>
-      </c>
-      <c r="I28" s="9">
-        <v>7.2969913298948086E-4</v>
-      </c>
-      <c r="J28" s="9">
-        <v>1553.4179999999999</v>
-      </c>
-      <c r="K28" s="9">
-        <v>36.9</v>
-      </c>
-      <c r="L28" s="9">
-        <v>1555.6690000000001</v>
-      </c>
-      <c r="M28" s="9">
-        <v>152.5</v>
-      </c>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
       <c r="N28" s="9"/>
-      <c r="O28" s="9">
-        <v>1549.6089999999999</v>
-      </c>
-      <c r="P28" s="9">
-        <f t="shared" si="0"/>
-        <v>-0.3910000000000764</v>
-      </c>
-      <c r="Q28" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="R28" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="S28" s="7">
-        <v>0.56699999999999995</v>
-      </c>
-      <c r="T28" s="7">
-        <v>1550.114</v>
-      </c>
-      <c r="U28" s="9">
-        <v>0.504</v>
-      </c>
-      <c r="V28" s="9">
-        <v>0</v>
-      </c>
-      <c r="W28" s="9">
-        <v>0.56699999999999995</v>
-      </c>
-      <c r="X28" s="9">
-        <v>1549.1</v>
-      </c>
-      <c r="Y28" s="9">
-        <v>0.50900000000000001</v>
-      </c>
-      <c r="Z28" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="AA28" s="9">
-        <v>0.56699999999999995</v>
-      </c>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+      <c r="AA28" s="9"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E29" s="9">
-        <v>1545.338</v>
-      </c>
-      <c r="F29" s="9">
-        <v>38</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="H29" s="9">
-        <v>0.69071365512716099</v>
-      </c>
-      <c r="I29" s="9">
-        <v>3.0002727548890111E-3</v>
-      </c>
-      <c r="J29" s="9">
-        <v>1553.4390000000001</v>
-      </c>
-      <c r="K29" s="9">
-        <v>37.299999999999997</v>
-      </c>
-      <c r="L29" s="9">
-        <v>1555.4469999999999</v>
-      </c>
-      <c r="M29" s="9">
-        <v>150.5</v>
-      </c>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
       <c r="N29" s="9"/>
-      <c r="O29" s="9">
-        <v>1549.9469999999999</v>
-      </c>
-      <c r="P29" s="9">
-        <f t="shared" si="0"/>
-        <v>-5.3000000000110958E-2</v>
-      </c>
-      <c r="Q29" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="R29" s="7">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="S29" s="7">
-        <v>0.59399999999999997</v>
-      </c>
-      <c r="T29" s="7">
-        <v>1550.4659999999999</v>
-      </c>
-      <c r="U29" s="9">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="V29" s="9">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="W29" s="9">
-        <v>0.59499999999999997</v>
-      </c>
-      <c r="X29" s="9">
-        <v>1549.4490000000001</v>
-      </c>
-      <c r="Y29" s="9">
-        <v>0.499</v>
-      </c>
-      <c r="Z29" s="9">
-        <v>2E-3</v>
-      </c>
-      <c r="AA29" s="9">
-        <v>0.59</v>
-      </c>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="Z29" s="9"/>
+      <c r="AA29" s="9"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E30" s="9">
-        <v>1545.107</v>
-      </c>
-      <c r="F30" s="9">
-        <v>30.6</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="H30" s="9">
-        <v>0.66031008141003145</v>
-      </c>
-      <c r="I30" s="9">
-        <v>3.1039609800700418E-3</v>
-      </c>
-      <c r="J30" s="9">
-        <v>1553.402</v>
-      </c>
-      <c r="K30" s="9">
-        <v>30.7</v>
-      </c>
-      <c r="L30" s="9">
-        <v>1555.4970000000001</v>
-      </c>
-      <c r="M30" s="9">
-        <v>149.4</v>
-      </c>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
       <c r="N30" s="9"/>
-      <c r="O30" s="9">
-        <v>1549.92</v>
-      </c>
-      <c r="P30" s="9">
-        <f t="shared" si="0"/>
-        <v>-7.999999999992724E-2</v>
-      </c>
-      <c r="Q30" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="R30" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="S30" s="7">
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="T30" s="7">
-        <v>1550.479</v>
-      </c>
-      <c r="U30" s="9">
-        <v>0.55800000000000005</v>
-      </c>
-      <c r="V30" s="9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="W30" s="9">
-        <v>0.56899999999999995</v>
-      </c>
-      <c r="X30" s="9">
-        <v>1549.385</v>
-      </c>
-      <c r="Y30" s="9">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="Z30" s="9">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="AA30" s="9">
-        <v>0.56699999999999995</v>
-      </c>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="9"/>
+      <c r="Z30" s="9"/>
+      <c r="AA30" s="9"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" s="9">
-        <v>1545.2629999999999</v>
-      </c>
-      <c r="F31" s="9">
-        <v>40.4</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="H31" s="9">
-        <v>0.60615219092581751</v>
-      </c>
-      <c r="I31" s="9">
-        <v>2.0925436699599231E-3</v>
-      </c>
-      <c r="J31" s="9">
-        <v>1553.405</v>
-      </c>
-      <c r="K31" s="9">
-        <v>36.6</v>
-      </c>
-      <c r="L31" s="9">
-        <v>1555.722</v>
-      </c>
-      <c r="M31" s="9">
-        <v>136.19999999999999</v>
-      </c>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
       <c r="N31" s="9"/>
-      <c r="O31" s="9">
-        <v>1549.895</v>
-      </c>
-      <c r="P31" s="9">
-        <f t="shared" si="0"/>
-        <v>-0.10500000000001819</v>
-      </c>
-      <c r="Q31" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="R31" s="7">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="S31" s="7">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="T31" s="7">
-        <v>1550.3889999999999</v>
-      </c>
-      <c r="U31" s="9">
-        <v>0.49399999999999999</v>
-      </c>
-      <c r="V31" s="9">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="W31" s="9">
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="X31" s="9">
-        <v>1549.4090000000001</v>
-      </c>
-      <c r="Y31" s="9">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="Z31" s="9">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="AA31" s="9">
-        <v>0.54400000000000004</v>
-      </c>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E32" s="9">
-        <v>1545.1690000000001</v>
-      </c>
-      <c r="F32" s="9">
-        <v>41.9</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="H32" s="9">
-        <v>0.66703417181252211</v>
-      </c>
-      <c r="I32" s="9">
-        <v>5.1771627854577673E-3</v>
-      </c>
-      <c r="J32" s="9">
-        <v>1553.403</v>
-      </c>
-      <c r="K32" s="9">
-        <v>42.2</v>
-      </c>
-      <c r="L32" s="9">
-        <v>1555.153</v>
-      </c>
-      <c r="M32" s="9">
-        <v>133.19999999999999</v>
-      </c>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
       <c r="N32" s="9"/>
-      <c r="O32" s="9">
-        <v>1549.665</v>
-      </c>
-      <c r="P32" s="9">
-        <f t="shared" si="0"/>
-        <v>-0.33500000000003638</v>
-      </c>
-      <c r="Q32" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="R32" s="7">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="S32" s="7">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="T32" s="7">
-        <v>1550.1469999999999</v>
-      </c>
-      <c r="U32" s="9">
-        <v>0.48299999999999998</v>
-      </c>
-      <c r="V32" s="9">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="W32" s="9">
-        <v>0.56200000000000006</v>
-      </c>
-      <c r="X32" s="9">
-        <v>1549.143</v>
-      </c>
-      <c r="Y32" s="9">
-        <v>0.52200000000000002</v>
-      </c>
-      <c r="Z32" s="9">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="AA32" s="9">
-        <v>0.56499999999999995</v>
-      </c>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="9"/>
+      <c r="Z32" s="9"/>
+      <c r="AA32" s="9"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33" s="9">
-        <v>1545.1489999999999</v>
-      </c>
-      <c r="F33" s="9">
-        <v>48.5</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="H33" s="9">
-        <v>0.67009452023517746</v>
-      </c>
-      <c r="I33" s="9">
-        <v>4.9797237124948879E-3</v>
-      </c>
-      <c r="J33" s="9">
-        <v>1553.3979999999999</v>
-      </c>
-      <c r="K33" s="9">
-        <v>44.4</v>
-      </c>
-      <c r="L33" s="9">
-        <v>1554.9849999999999</v>
-      </c>
-      <c r="M33" s="9">
-        <v>139.5</v>
-      </c>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
       <c r="N33" s="9"/>
-      <c r="O33" s="9">
-        <v>1549.652</v>
-      </c>
-      <c r="P33" s="9">
-        <f t="shared" si="0"/>
-        <v>-0.34799999999995634</v>
-      </c>
-      <c r="Q33" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="R33" s="7">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="S33" s="7">
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="T33" s="7">
-        <v>1550.1569999999999</v>
-      </c>
-      <c r="U33" s="9">
-        <v>0.505</v>
-      </c>
-      <c r="V33" s="9">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="W33" s="9">
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="X33" s="9">
-        <v>1549.1130000000001</v>
-      </c>
-      <c r="Y33" s="9">
-        <v>0.53900000000000003</v>
-      </c>
-      <c r="Z33" s="9">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AA33" s="9">
-        <v>0.58299999999999996</v>
-      </c>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="9"/>
+      <c r="X33" s="9"/>
+      <c r="Y33" s="9"/>
+      <c r="Z33" s="9"/>
+      <c r="AA33" s="9"/>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E34" s="9">
-        <v>1545.2349999999999</v>
-      </c>
-      <c r="F34" s="9">
-        <v>47.4</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H34" s="9">
-        <v>0.60688014988285743</v>
-      </c>
-      <c r="I34" s="9">
-        <v>3.1288580157706752E-4</v>
-      </c>
-      <c r="J34" s="9">
-        <v>1553.395</v>
-      </c>
-      <c r="K34" s="9">
-        <v>46.3</v>
-      </c>
-      <c r="L34" s="9">
-        <v>1555.443</v>
-      </c>
-      <c r="M34" s="9">
-        <v>149.5</v>
-      </c>
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
       <c r="N34" s="9"/>
-      <c r="O34" s="9">
-        <v>1550.076</v>
-      </c>
-      <c r="P34" s="9">
-        <f t="shared" si="0"/>
-        <v>7.6000000000021828E-2</v>
-      </c>
-      <c r="Q34" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="R34" s="7">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="S34" s="7">
-        <v>0.54</v>
-      </c>
-      <c r="T34" s="7">
-        <v>1550.5730000000001</v>
-      </c>
-      <c r="U34" s="9">
-        <v>0.497</v>
-      </c>
-      <c r="V34" s="9">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="W34" s="9">
-        <v>0.54100000000000004</v>
-      </c>
-      <c r="X34" s="9">
-        <v>1549.6030000000001</v>
-      </c>
-      <c r="Y34" s="9">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="Z34" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AA34" s="9">
-        <v>0.54200000000000004</v>
-      </c>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="9"/>
+      <c r="V34" s="9"/>
+      <c r="W34" s="9"/>
+      <c r="X34" s="9"/>
+      <c r="Y34" s="9"/>
+      <c r="Z34" s="9"/>
+      <c r="AA34" s="9"/>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E35" s="9">
-        <v>1545.2670000000001</v>
-      </c>
-      <c r="F35" s="9">
-        <v>46.3</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="H35" s="9">
-        <v>0.60530640350468301</v>
-      </c>
-      <c r="I35" s="9">
-        <v>8.7427598896283598E-4</v>
-      </c>
-      <c r="J35" s="9">
-        <v>1553.413</v>
-      </c>
-      <c r="K35" s="9">
-        <v>46</v>
-      </c>
-      <c r="L35" s="9">
-        <v>1554.8789999999999</v>
-      </c>
-      <c r="M35" s="9">
-        <v>150</v>
-      </c>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
       <c r="N35" s="9"/>
-      <c r="O35" s="9">
-        <v>1549.778</v>
-      </c>
-      <c r="P35" s="9">
-        <f t="shared" si="0"/>
-        <v>-0.22199999999997999</v>
-      </c>
-      <c r="Q35" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="R35" s="7">
-        <v>2E-3</v>
-      </c>
-      <c r="S35" s="7">
-        <v>0.54</v>
-      </c>
-      <c r="T35" s="7">
-        <v>1550.29</v>
-      </c>
-      <c r="U35" s="9">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="V35" s="9">
-        <v>0</v>
-      </c>
-      <c r="W35" s="9">
-        <v>0.54</v>
-      </c>
-      <c r="X35" s="9">
-        <v>1549.2460000000001</v>
-      </c>
-      <c r="Y35" s="9">
-        <v>0.53200000000000003</v>
-      </c>
-      <c r="Z35" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA35" s="9">
-        <v>0.54</v>
-      </c>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9"/>
+      <c r="W35" s="9"/>
+      <c r="X35" s="9"/>
+      <c r="Y35" s="9"/>
+      <c r="Z35" s="9"/>
+      <c r="AA35" s="9"/>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E36" s="9">
-        <v>1545.145</v>
-      </c>
-      <c r="F36" s="9">
-        <v>26.7</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H36" s="9">
-        <v>0.58943015108104813</v>
-      </c>
-      <c r="I36" s="9">
-        <v>8.895573701011017E-4</v>
-      </c>
-      <c r="J36" s="9">
-        <v>1553.405</v>
-      </c>
-      <c r="K36" s="9">
-        <v>26.7</v>
-      </c>
-      <c r="L36" s="9">
-        <v>1555.3810000000001</v>
-      </c>
-      <c r="M36" s="9">
-        <v>26.7</v>
-      </c>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
       <c r="N36" s="9"/>
       <c r="O36" s="9"/>
-      <c r="P36" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P36" s="9"/>
       <c r="Q36" s="7"/>
       <c r="R36" s="7"/>
       <c r="S36" s="7"/>
@@ -3687,51 +1572,22 @@
       <c r="AA36" s="9"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E37" s="9">
-        <v>1545.2139999999999</v>
-      </c>
-      <c r="F37" s="9">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="H37" s="9">
-        <v>0.64554958728623779</v>
-      </c>
-      <c r="I37" s="9">
-        <v>2.8179300866213448E-3</v>
-      </c>
-      <c r="J37" s="9">
-        <v>1553.4069999999999</v>
-      </c>
-      <c r="K37" s="9">
-        <v>35.1</v>
-      </c>
-      <c r="L37" s="9">
-        <v>1555.4960000000001</v>
-      </c>
-      <c r="M37" s="9">
-        <v>154.6</v>
-      </c>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
       <c r="N37" s="9"/>
       <c r="O37" s="9"/>
-      <c r="P37" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P37" s="9"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="7"/>
       <c r="S37" s="7"/>
@@ -3745,51 +1601,22 @@
       <c r="AA37" s="9"/>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E38" s="9">
-        <v>1544.9949999999999</v>
-      </c>
-      <c r="F38" s="9">
-        <v>32.4</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="H38" s="9">
-        <v>0.65103196382598538</v>
-      </c>
-      <c r="I38" s="9">
-        <v>5.2332120003484306E-4</v>
-      </c>
-      <c r="J38" s="9">
-        <v>1553.395</v>
-      </c>
-      <c r="K38" s="9">
-        <v>32.1</v>
-      </c>
-      <c r="L38" s="9">
-        <v>1555.0930000000001</v>
-      </c>
-      <c r="M38" s="9">
-        <v>147.30000000000001</v>
-      </c>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
-      <c r="P38" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P38" s="9"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="7"/>
       <c r="S38" s="7"/>
@@ -3803,51 +1630,22 @@
       <c r="AA38" s="9"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E39" s="9">
-        <v>1545.2260000000001</v>
-      </c>
-      <c r="F39" s="9">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="H39" s="9">
-        <v>0.60817457103252104</v>
-      </c>
-      <c r="I39" s="9">
-        <v>3.3122778606866632E-3</v>
-      </c>
-      <c r="J39" s="9">
-        <v>1553.4059999999999</v>
-      </c>
-      <c r="K39" s="9">
-        <v>38.6</v>
-      </c>
-      <c r="L39" s="9">
-        <v>1555.807</v>
-      </c>
-      <c r="M39" s="9">
-        <v>148.30000000000001</v>
-      </c>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
       <c r="N39" s="9"/>
       <c r="O39" s="9"/>
-      <c r="P39" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P39" s="9"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7"/>
       <c r="S39" s="7"/>
@@ -3861,51 +1659,22 @@
       <c r="AA39" s="9"/>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E40" s="9">
-        <v>1545.2570000000001</v>
-      </c>
-      <c r="F40" s="9">
-        <v>39.200000000000003</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="H40" s="9">
-        <v>0.61124090243057594</v>
-      </c>
-      <c r="I40" s="9">
-        <v>3.0069234765051078E-3</v>
-      </c>
-      <c r="J40" s="9">
-        <v>1553.422</v>
-      </c>
-      <c r="K40" s="9">
-        <v>51.8</v>
-      </c>
-      <c r="L40" s="9">
-        <v>1555.289</v>
-      </c>
-      <c r="M40" s="9">
-        <v>152.80000000000001</v>
-      </c>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
       <c r="N40" s="9"/>
       <c r="O40" s="9"/>
-      <c r="P40" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P40" s="9"/>
       <c r="Q40" s="7"/>
       <c r="R40" s="7"/>
       <c r="S40" s="7"/>
@@ -3919,51 +1688,22 @@
       <c r="AA40" s="9"/>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E41" s="9">
-        <v>1545.2360000000001</v>
-      </c>
-      <c r="F41" s="9">
-        <v>42.2</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="H41" s="9">
-        <v>0.61512543234611905</v>
-      </c>
-      <c r="I41" s="9">
-        <v>1.504154465465035E-3</v>
-      </c>
-      <c r="J41" s="9">
-        <v>1553.4090000000001</v>
-      </c>
-      <c r="K41" s="9">
-        <v>41.1</v>
-      </c>
-      <c r="L41" s="9">
-        <v>1555.0219999999999</v>
-      </c>
-      <c r="M41" s="9">
-        <v>152.4</v>
-      </c>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
-      <c r="P41" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P41" s="9"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="7"/>
       <c r="S41" s="7"/>
@@ -3977,51 +1717,22 @@
       <c r="AA41" s="9"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E42" s="9">
-        <v>1545.011</v>
-      </c>
-      <c r="F42" s="9">
-        <v>41.4</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="H42" s="9">
-        <v>0.68190175872857239</v>
-      </c>
-      <c r="I42" s="9">
-        <v>3.5434297706160578E-4</v>
-      </c>
-      <c r="J42" s="9">
-        <v>1553.3789999999999</v>
-      </c>
-      <c r="K42" s="9">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="L42" s="9">
-        <v>1555.18</v>
-      </c>
-      <c r="M42" s="9">
-        <v>155.1</v>
-      </c>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
-      <c r="P42" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P42" s="9"/>
       <c r="Q42" s="7"/>
       <c r="R42" s="7"/>
       <c r="S42" s="7"/>
@@ -4035,51 +1746,22 @@
       <c r="AA42" s="9"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E43" s="9">
-        <v>1545.0509999999999</v>
-      </c>
-      <c r="F43" s="9">
-        <v>42.1</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="H43" s="9">
-        <v>0.65512294522539227</v>
-      </c>
-      <c r="I43" s="9">
-        <v>4.0978581741910602E-3</v>
-      </c>
-      <c r="J43" s="9">
-        <v>1553.3679999999999</v>
-      </c>
-      <c r="K43" s="9">
-        <v>40.700000000000003</v>
-      </c>
-      <c r="L43" s="9">
-        <v>1555.307</v>
-      </c>
-      <c r="M43" s="9">
-        <v>151.6</v>
-      </c>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
       <c r="N43" s="9"/>
       <c r="O43" s="9"/>
-      <c r="P43" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P43" s="9"/>
       <c r="Q43" s="7"/>
       <c r="R43" s="7"/>
       <c r="S43" s="7"/>
@@ -4093,51 +1775,22 @@
       <c r="AA43" s="9"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E44" s="9">
-        <v>1549.7090000000001</v>
-      </c>
-      <c r="F44" s="9">
-        <v>34.1</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="H44" s="9">
-        <v>0.70513586831372155</v>
-      </c>
-      <c r="I44" s="9">
-        <v>4.7496385011652356</v>
-      </c>
-      <c r="J44" s="9">
-        <v>1553.3879999999999</v>
-      </c>
-      <c r="K44" s="9">
-        <v>33.9</v>
-      </c>
-      <c r="L44" s="9">
-        <v>1555.481</v>
-      </c>
-      <c r="M44" s="9">
-        <v>148</v>
-      </c>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
       <c r="N44" s="9"/>
       <c r="O44" s="9"/>
-      <c r="P44" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P44" s="9"/>
       <c r="Q44" s="7"/>
       <c r="R44" s="7"/>
       <c r="S44" s="7"/>
@@ -4151,51 +1804,22 @@
       <c r="AA44" s="9"/>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E45" s="9">
-        <v>1545.1120000000001</v>
-      </c>
-      <c r="F45" s="9">
-        <v>39.9</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="H45" s="9">
-        <v>0.65727828330702265</v>
-      </c>
-      <c r="I45" s="9">
-        <v>2.691441775596104E-3</v>
-      </c>
-      <c r="J45" s="9">
-        <v>1553.3620000000001</v>
-      </c>
-      <c r="K45" s="9">
-        <v>38.799999999999997</v>
-      </c>
-      <c r="L45" s="9">
-        <v>1555.3050000000001</v>
-      </c>
-      <c r="M45" s="9">
-        <v>152</v>
-      </c>
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
-      <c r="P45" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P45" s="9"/>
       <c r="Q45" s="7"/>
       <c r="R45" s="7"/>
       <c r="S45" s="7"/>
@@ -4209,51 +1833,22 @@
       <c r="AA45" s="9"/>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E46" s="9">
-        <v>1545.261</v>
-      </c>
-      <c r="F46" s="9">
-        <v>43.2</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="H46" s="9">
-        <v>0.68165064278284959</v>
-      </c>
-      <c r="I46" s="9">
-        <v>3.2722553542043902E-3</v>
-      </c>
-      <c r="J46" s="9">
-        <v>1553.4010000000001</v>
-      </c>
-      <c r="K46" s="9">
-        <v>41.5</v>
-      </c>
-      <c r="L46" s="9">
-        <v>1555.3330000000001</v>
-      </c>
-      <c r="M46" s="9">
-        <v>149.1</v>
-      </c>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
-      <c r="P46" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P46" s="9"/>
       <c r="Q46" s="7"/>
       <c r="R46" s="7"/>
       <c r="S46" s="7"/>
@@ -4282,10 +1877,7 @@
       <c r="M47" s="9"/>
       <c r="N47" s="9"/>
       <c r="O47" s="9"/>
-      <c r="P47" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P47" s="9"/>
       <c r="Q47" s="7"/>
       <c r="R47" s="7"/>
       <c r="S47" s="7"/>
@@ -4314,10 +1906,7 @@
       <c r="M48" s="9"/>
       <c r="N48" s="9"/>
       <c r="O48" s="9"/>
-      <c r="P48" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P48" s="9"/>
       <c r="Q48" s="7"/>
       <c r="R48" s="7"/>
       <c r="S48" s="7"/>
@@ -4346,10 +1935,7 @@
       <c r="M49" s="9"/>
       <c r="N49" s="9"/>
       <c r="O49" s="9"/>
-      <c r="P49" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="P49" s="9"/>
       <c r="Q49" s="7"/>
       <c r="R49" s="7"/>
       <c r="S49" s="7"/>
@@ -4379,7 +1965,7 @@
       <c r="N50" s="9"/>
       <c r="O50" s="9"/>
       <c r="P50" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="P50:P68" si="0">IF(O50,O50-1550,"-")</f>
         <v>-</v>
       </c>
       <c r="Q50" s="7"/>
@@ -33659,7 +31245,7 @@
       <c r="N965" s="9"/>
       <c r="O965" s="9"/>
       <c r="P965" s="9" t="str">
-        <f t="shared" ref="P965:P1028" si="15">IF(O965,O965-1550,"-")</f>
+        <f t="shared" ref="P965:P1007" si="15">IF(O965,O965-1550,"-")</f>
         <v>-</v>
       </c>
       <c r="Q965" s="7"/>

</xml_diff>